<commit_message>
Added new python files to merge json files together and ensured that json file is cleaned.
</commit_message>
<xml_diff>
--- a/Code/Youtube Data/video_ids.xlsx
+++ b/Code/Youtube Data/video_ids.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rusha\RD Documents\Rushabh's career\Computer Science\University\Year\Year 3\Semester 1\Web and Cloud Based Security\COMP-3226-Web-and-Cloud-Based-Security-\Code\Youtube Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A21A4A0-8245-4B7D-93B6-4B3804B43359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B6BEB9-8A6F-412D-A533-16233CFF08D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34485" yWindow="4740" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="344">
   <si>
     <t>videoID</t>
   </si>
@@ -768,6 +768,303 @@
   </si>
   <si>
     <t>Ha80ZaecGkQ</t>
+  </si>
+  <si>
+    <t>JAjxq93njvs</t>
+  </si>
+  <si>
+    <t>Bi0taCrL22Q</t>
+  </si>
+  <si>
+    <t>Vkack7OKYjQ</t>
+  </si>
+  <si>
+    <t>o7FmGwoDJvc</t>
+  </si>
+  <si>
+    <t>jJUvn-i73zI</t>
+  </si>
+  <si>
+    <t>1AMFwO7BGW8</t>
+  </si>
+  <si>
+    <t>8DkcTriimSM</t>
+  </si>
+  <si>
+    <t>G5iGJHVtFqs</t>
+  </si>
+  <si>
+    <t>Mh5dKiiZRlg</t>
+  </si>
+  <si>
+    <t>3he4lvoghMg</t>
+  </si>
+  <si>
+    <t>xTsREJ6KEfg</t>
+  </si>
+  <si>
+    <t>kaqxOKmq0ZI</t>
+  </si>
+  <si>
+    <t>muT3_bTXR_w</t>
+  </si>
+  <si>
+    <t>5tQPftbhCVo</t>
+  </si>
+  <si>
+    <t>tivtBueDg_c</t>
+  </si>
+  <si>
+    <t>k7PmttZtFU0</t>
+  </si>
+  <si>
+    <t>m5zhPegPUc8</t>
+  </si>
+  <si>
+    <t>Su_SV29obhE</t>
+  </si>
+  <si>
+    <t>UmTBOw5ITeU</t>
+  </si>
+  <si>
+    <t>Er2IIYpGgS0</t>
+  </si>
+  <si>
+    <t>ouPsgmEKyww</t>
+  </si>
+  <si>
+    <t>19IdcJU8524</t>
+  </si>
+  <si>
+    <t>G5_YyZUOQL8</t>
+  </si>
+  <si>
+    <t>jCIf07qU_mQ</t>
+  </si>
+  <si>
+    <t>xhIFmxslJCQ</t>
+  </si>
+  <si>
+    <t>L3ibkV6t0NM</t>
+  </si>
+  <si>
+    <t>4vfIC0dZ8jM</t>
+  </si>
+  <si>
+    <t>MrNcHCki8mE</t>
+  </si>
+  <si>
+    <t>YDdN4vm_59c</t>
+  </si>
+  <si>
+    <t>u6Q8ywGzkAI</t>
+  </si>
+  <si>
+    <t>DdPWX4RqDOY</t>
+  </si>
+  <si>
+    <t>YSrjyXqA5cM</t>
+  </si>
+  <si>
+    <t>jn73kYaLmKM</t>
+  </si>
+  <si>
+    <t>2HS3sFyywnM</t>
+  </si>
+  <si>
+    <t>O6mZnetxUX8</t>
+  </si>
+  <si>
+    <t>vyB_2BnouRs</t>
+  </si>
+  <si>
+    <t>x-axYKSh-jc</t>
+  </si>
+  <si>
+    <t>2nUGLtfiTbk</t>
+  </si>
+  <si>
+    <t>qb6UuECcPV0</t>
+  </si>
+  <si>
+    <t>YpUgnlZkPEI</t>
+  </si>
+  <si>
+    <t>WMSpjDc8zH8</t>
+  </si>
+  <si>
+    <t>sxn5n89S7Xw</t>
+  </si>
+  <si>
+    <t>VKJZ4PCWgY8</t>
+  </si>
+  <si>
+    <t>Bd2fE3YO7Aw</t>
+  </si>
+  <si>
+    <t>4SL11QJZzCI</t>
+  </si>
+  <si>
+    <t>0ONPlWHl9Gk</t>
+  </si>
+  <si>
+    <t>L-PkACES1qc</t>
+  </si>
+  <si>
+    <t>o8hO9R_Xs7Q</t>
+  </si>
+  <si>
+    <t>Qs0KZwhKdwo</t>
+  </si>
+  <si>
+    <t>moSE2_ur994</t>
+  </si>
+  <si>
+    <t>BlO34GiRoJ0</t>
+  </si>
+  <si>
+    <t>JM1S2ZkNVrQ</t>
+  </si>
+  <si>
+    <t>L4B7z8dHDRc</t>
+  </si>
+  <si>
+    <t>cKW-pp1pprg</t>
+  </si>
+  <si>
+    <t>sWVPnyyLnFw</t>
+  </si>
+  <si>
+    <t>DPDUDPCttfc</t>
+  </si>
+  <si>
+    <t>OGiBcHF-wOU</t>
+  </si>
+  <si>
+    <t>VkqiSzoVtUA</t>
+  </si>
+  <si>
+    <t>Id1rwD0RU5k</t>
+  </si>
+  <si>
+    <t>AHIlxaPZd5w</t>
+  </si>
+  <si>
+    <t>mxWIy8q_vQw</t>
+  </si>
+  <si>
+    <t>ro5arbsZfMs</t>
+  </si>
+  <si>
+    <t>goCGfcCjtSo</t>
+  </si>
+  <si>
+    <t>MAm0RLQpYas</t>
+  </si>
+  <si>
+    <t>qKKNbYv3LrM</t>
+  </si>
+  <si>
+    <t>vO4QeHR9SXM</t>
+  </si>
+  <si>
+    <t>w-253j0BjLk</t>
+  </si>
+  <si>
+    <t>hddRxBhGiMI</t>
+  </si>
+  <si>
+    <t>YqKYpgZ9FWU</t>
+  </si>
+  <si>
+    <t>gTo-lPOGPdg</t>
+  </si>
+  <si>
+    <t>PzHZGefMx9Q</t>
+  </si>
+  <si>
+    <t>btFETPVpDcw</t>
+  </si>
+  <si>
+    <t>nSNkwIvlWJU</t>
+  </si>
+  <si>
+    <t>LWHMtkbCxd0</t>
+  </si>
+  <si>
+    <t>YJOmxjtG9IM</t>
+  </si>
+  <si>
+    <t>jEWaLRi_G60</t>
+  </si>
+  <si>
+    <t>GlUp3MCIQIk</t>
+  </si>
+  <si>
+    <t>OqGH_6mLQjI</t>
+  </si>
+  <si>
+    <t>S1ABZywPONY</t>
+  </si>
+  <si>
+    <t>eO6e0b4i93U</t>
+  </si>
+  <si>
+    <t>1CLhjDLUl4c</t>
+  </si>
+  <si>
+    <t>xDi_TTbk3-c</t>
+  </si>
+  <si>
+    <t>Z0L0xWZhYTE</t>
+  </si>
+  <si>
+    <t>t8rMgGSgHv0</t>
+  </si>
+  <si>
+    <t>sJj3q6njVbM</t>
+  </si>
+  <si>
+    <t>ImO6sDdYB8U</t>
+  </si>
+  <si>
+    <t>3Bi-0s8djNE</t>
+  </si>
+  <si>
+    <t>04kGIbHUIho</t>
+  </si>
+  <si>
+    <t>Y1E6R13YD1Y</t>
+  </si>
+  <si>
+    <t>7hTgjEzl4Bk</t>
+  </si>
+  <si>
+    <t>BW_MAa5L9lg</t>
+  </si>
+  <si>
+    <t>16RX6rKJle8</t>
+  </si>
+  <si>
+    <t>hN0xpuih8zo</t>
+  </si>
+  <si>
+    <t>mcTpep5uoZ8</t>
+  </si>
+  <si>
+    <t>uqv-oC-Izi8</t>
+  </si>
+  <si>
+    <t>_bhXh1KxVHc</t>
+  </si>
+  <si>
+    <t>nSI_2yvBAIU</t>
+  </si>
+  <si>
+    <t>8a5Z1Idf-Jo</t>
+  </si>
+  <si>
+    <t>dkf9LNwo2kM</t>
   </si>
 </sst>
 </file>
@@ -1130,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A251"/>
+  <dimension ref="A1:A351"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="L256" sqref="L256"/>
+    <sheetView tabSelected="1" topLeftCell="A306" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E311" sqref="E311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2396,6 +2693,506 @@
         <v>244</v>
       </c>
     </row>
+    <row r="252" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A252" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="253" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A253" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="254" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A254" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A255" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A256" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A257" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A258" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A259" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A260" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A261" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A262" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A263" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A264" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="265" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A265" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A266" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="267" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A267" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A268" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A269" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A270" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A271" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A272" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="273" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A273" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A274" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A275" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="276" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A276" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A277" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A278" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A279" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A280" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A281" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="282" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A282" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A283" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A284" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A285" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A286" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A287" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A288" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A289" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="290" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A290" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A291" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A292" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A293" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A294" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A295" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A296" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A297" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="298" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A298" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A299" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A300" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A301" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A302" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A303" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="304" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A304" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="305" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A305" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A306" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A307" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A308" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A309" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A310" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A311" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A312" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A313" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="314" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A314" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A315" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A316" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A317" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A318" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A319" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A320" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A321" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A322" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A323" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A324" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A325" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A326" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A327" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A328" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A329" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A330" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A331" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A332" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A333" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A334" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A335" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A336" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A337" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A338" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A339" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A340" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A341" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A342" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A343" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A344" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A345" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A346" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A347" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A348" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A349" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>343</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>